<commit_message>
change 'budget area' to 'priority area' throughout the code and data
</commit_message>
<xml_diff>
--- a/data/input-data/ontology.xlsx
+++ b/data/input-data/ontology.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15300" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="23940" windowHeight="12500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="81">
   <si>
     <t>Class</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -128,9 +128,6 @@
     <t>A type of Product that provides a process to identify the best Applicants to take part in a Project  or receive Funding for a specific innovation</t>
   </si>
   <si>
-    <t>Area</t>
-  </si>
-  <si>
     <t>A defined  segment of UK technology  knowledge and experience identified in the TSB Strategy and Delivery Plan for investment with a defined budgeted commitment. Also used as a division of  the internal organisation.</t>
   </si>
   <si>
@@ -233,9 +230,6 @@
     <t>activityCode</t>
   </si>
   <si>
-    <t>budgetArea</t>
-  </si>
-  <si>
     <t>product</t>
   </si>
   <si>
@@ -257,19 +251,28 @@
     <t>activity code</t>
   </si>
   <si>
-    <t>budget area</t>
-  </si>
-  <si>
     <t>http://www.w3.org/ns/legal#companyType</t>
   </si>
   <si>
     <t>http://www.w3.org/ns/legal#companyActivity</t>
   </si>
   <si>
-    <t>budgetSubArea</t>
-  </si>
-  <si>
-    <t>budget area subdivision</t>
+    <t>prioritySubArea</t>
+  </si>
+  <si>
+    <t>priority area subdivision</t>
+  </si>
+  <si>
+    <t>priorityArea</t>
+  </si>
+  <si>
+    <t>priority area</t>
+  </si>
+  <si>
+    <t>PriorityArea</t>
+  </si>
+  <si>
+    <t>Priority Area</t>
   </si>
 </sst>
 </file>
@@ -886,8 +889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -971,16 +974,16 @@
     </row>
     <row r="7" spans="1:4" ht="70">
       <c r="A7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>33</v>
-      </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -999,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1050,10 +1053,10 @@
     </row>
     <row r="3" spans="1:6" ht="26">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
@@ -1067,10 +1070,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -1081,7 +1084,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -1092,10 +1095,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
@@ -1109,7 +1112,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="4"/>
       <c r="E7" t="s">
@@ -1121,10 +1124,10 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="4"/>
       <c r="E8" t="s">
@@ -1133,10 +1136,10 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
@@ -1144,10 +1147,10 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -1155,10 +1158,10 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
         <v>13</v>
@@ -1166,10 +1169,10 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
@@ -1177,14 +1180,14 @@
     </row>
     <row r="13" spans="1:6" ht="17">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13"/>
       <c r="D13" s="8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -1192,27 +1195,27 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E14" t="s">
         <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="17">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
         <v>14</v>
@@ -1223,7 +1226,7 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -1234,7 +1237,7 @@
         <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
         <v>12</v>
@@ -1242,10 +1245,10 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E18" t="s">
         <v>12</v>
@@ -1256,7 +1259,7 @@
         <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E19" t="s">
         <v>12</v>
@@ -1267,7 +1270,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E20" t="s">
         <v>12</v>
@@ -1275,10 +1278,10 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" t="s">
         <v>12</v>
@@ -1286,10 +1289,10 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E22" t="s">
         <v>28</v>
@@ -1297,10 +1300,10 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E23" t="s">
         <v>28</v>
@@ -1308,10 +1311,10 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E24" t="s">
         <v>28</v>
@@ -1319,10 +1322,10 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E25" t="s">
         <v>28</v>
@@ -1330,10 +1333,10 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E26" t="s">
         <v>28</v>
@@ -1341,24 +1344,24 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B27" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E27" t="s">
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E28" t="s">
         <v>28</v>

</xml_diff>